<commit_message>
[HW] Add & Fix : DDR Schematic Page & Etc
</commit_message>
<xml_diff>
--- a/HW/Document/BOM/01_Required Part List/Main Part List of BeagleBoneBlack.xlsx
+++ b/HW/Document/BOM/01_Required Part List/Main Part List of BeagleBoneBlack.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ArkX\N2_Project\Year_2025\Sitara-Project\HW\Document\BOM\01_Required Part List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE4189B-C92C-4D67-B1FE-B0D0FAB64710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9707F75A-2738-431A-B522-3386987B4202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BeagleBoneBlack's Main Part" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="183" formatCode="\$#,##0.00"/>
-    <numFmt numFmtId="184" formatCode="\$#,##0.000"/>
-    <numFmt numFmtId="185" formatCode="#,##0_ "/>
-    <numFmt numFmtId="187" formatCode="\$#,##0"/>
+    <numFmt numFmtId="176" formatCode="\$#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="\$#,##0.000"/>
+    <numFmt numFmtId="178" formatCode="#,##0_ "/>
+    <numFmt numFmtId="179" formatCode="\$#,##0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -630,7 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,91 +653,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="185" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="183" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="185" fontId="7" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="6" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="6" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="6" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="6" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -746,13 +707,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="185" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="6" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -767,44 +728,80 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="185" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="6" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="7" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1095,7 +1092,7 @@
   <dimension ref="B2:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1116,77 +1113,77 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="35.25" customHeight="1">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="10"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="48"/>
     </row>
     <row r="3" spans="2:17" ht="23.25" customHeight="1">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="57"/>
+      <c r="E3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="12" t="s">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="M3" s="16"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="14" t="s">
+      <c r="M3" s="56"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="43" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:17" ht="23.25" customHeight="1">
-      <c r="B4" s="15"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="44"/>
+      <c r="C4" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="2" t="s">
         <v>70</v>
       </c>
@@ -1205,9 +1202,9 @@
       <c r="N4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
     </row>
     <row r="5" spans="2:17">
       <c r="B5" s="3">
@@ -1231,27 +1228,27 @@
       <c r="H5" s="3">
         <v>1</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="17">
         <v>305</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="18">
         <v>2.2305000000000001</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="19">
         <f>H5*J5</f>
         <v>2.2305000000000001</v>
       </c>
-      <c r="L5" s="20">
+      <c r="L5" s="12">
         <v>2259</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="9">
         <v>5.2</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="15">
         <f>H5*M5</f>
         <v>5.2</v>
       </c>
-      <c r="O5" s="23">
+      <c r="O5" s="15">
         <f>K5</f>
         <v>2.2305000000000001</v>
       </c>
@@ -1282,27 +1279,27 @@
       <c r="H6" s="3">
         <v>1</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="17">
         <v>65</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="18">
         <v>1.125</v>
       </c>
-      <c r="K6" s="32">
+      <c r="K6" s="19">
         <f t="shared" ref="K6:K20" si="0">H6*J6</f>
         <v>1.125</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="12">
         <v>0</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="9">
         <v>1.52</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="15">
         <f t="shared" ref="N6:N20" si="1">H6*M6</f>
         <v>1.52</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="15">
         <f>K6</f>
         <v>1.125</v>
       </c>
@@ -1332,27 +1329,27 @@
       <c r="H7" s="3">
         <v>1</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="20">
         <v>11337</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7" s="21">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="K7" s="32">
+      <c r="K7" s="19">
         <f t="shared" si="0"/>
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="L7" s="21">
+      <c r="L7" s="13">
         <v>110269</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="10">
         <v>0.1</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="15">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="O7" s="23">
+      <c r="O7" s="15">
         <f>K7</f>
         <v>4.7899999999999998E-2</v>
       </c>
@@ -1383,27 +1380,27 @@
       <c r="H8" s="3">
         <v>1</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="20">
         <v>186</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="21">
         <v>0.35399999999999998</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K8" s="19">
         <f t="shared" si="0"/>
         <v>0.35399999999999998</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="13">
         <v>23303</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="10">
         <v>0.5</v>
       </c>
-      <c r="N8" s="23">
+      <c r="N8" s="15">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="O8" s="23">
+      <c r="O8" s="15">
         <f>K8</f>
         <v>0.35399999999999998</v>
       </c>
@@ -1434,27 +1431,27 @@
       <c r="H9" s="3">
         <v>1</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="20">
         <v>1456</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="21">
         <v>6.5100000000000005E-2</v>
       </c>
-      <c r="K9" s="32">
+      <c r="K9" s="19">
         <f t="shared" si="0"/>
         <v>6.5100000000000005E-2</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="13">
         <v>41948</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="10">
         <v>0.1</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="15">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="O9" s="23">
+      <c r="O9" s="15">
         <f>K9</f>
         <v>6.5100000000000005E-2</v>
       </c>
@@ -1464,48 +1461,48 @@
       <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="2:17">
-      <c r="B10" s="44">
+      <c r="B10" s="31">
         <v>6</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="F10" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="31">
         <v>1</v>
       </c>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="47" t="s">
+      <c r="J10" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="48" t="s">
+      <c r="K10" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="46" t="s">
+      <c r="L10" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="47" t="s">
+      <c r="M10" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="48" t="s">
+      <c r="N10" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="48"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="45" t="s">
+      <c r="O10" s="35"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="32" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1531,27 +1528,27 @@
       <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="20">
         <v>219</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="21">
         <v>12.218999999999999</v>
       </c>
-      <c r="K11" s="32">
+      <c r="K11" s="19">
         <f t="shared" si="0"/>
         <v>12.218999999999999</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="13">
         <v>149</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="10">
         <v>18.79</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="15">
         <f t="shared" si="1"/>
         <v>18.79</v>
       </c>
-      <c r="O11" s="23">
+      <c r="O11" s="15">
         <f>K11</f>
         <v>12.218999999999999</v>
       </c>
@@ -1582,27 +1579,27 @@
       <c r="H12" s="3">
         <v>1</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="20">
         <v>3266</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="21">
         <v>0.34139999999999998</v>
       </c>
-      <c r="K12" s="32">
+      <c r="K12" s="19">
         <f t="shared" si="0"/>
         <v>0.34139999999999998</v>
       </c>
-      <c r="L12" s="21">
+      <c r="L12" s="13">
         <v>14155</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="10">
         <v>0.45</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="15">
         <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
-      <c r="O12" s="23">
+      <c r="O12" s="15">
         <f>K12</f>
         <v>0.34139999999999998</v>
       </c>
@@ -1633,27 +1630,27 @@
       <c r="H13" s="3">
         <v>1</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="14">
         <v>0</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="11">
         <v>0.96</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="15">
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
-      <c r="L13" s="35">
+      <c r="L13" s="22">
         <v>6079</v>
       </c>
-      <c r="M13" s="36">
+      <c r="M13" s="23">
         <v>0.96</v>
       </c>
-      <c r="N13" s="32">
+      <c r="N13" s="19">
         <f t="shared" si="1"/>
         <v>0.96</v>
       </c>
-      <c r="O13" s="23">
+      <c r="O13" s="15">
         <f>N13</f>
         <v>0.96</v>
       </c>
@@ -1684,27 +1681,27 @@
       <c r="H14" s="3">
         <v>2</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="20">
         <v>224</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="21">
         <v>0.16969999999999999</v>
       </c>
-      <c r="K14" s="32">
+      <c r="K14" s="19">
         <f t="shared" si="0"/>
         <v>0.33939999999999998</v>
       </c>
-      <c r="L14" s="21">
+      <c r="L14" s="13">
         <v>27863</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="10">
         <v>0.69</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="15">
         <f t="shared" si="1"/>
         <v>1.38</v>
       </c>
-      <c r="O14" s="23">
+      <c r="O14" s="15">
         <f>K14</f>
         <v>0.33939999999999998</v>
       </c>
@@ -1714,51 +1711,51 @@
       <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="2:17">
-      <c r="B15" s="44">
+      <c r="B15" s="31">
         <v>11</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="45" t="s">
+      <c r="F15" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="44" t="s">
+      <c r="G15" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="44">
+      <c r="H15" s="31">
         <v>1</v>
       </c>
-      <c r="I15" s="49" t="s">
+      <c r="I15" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="50" t="s">
+      <c r="J15" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="48" t="s">
+      <c r="K15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="49">
+      <c r="L15" s="36">
         <v>259</v>
       </c>
-      <c r="M15" s="50">
+      <c r="M15" s="37">
         <v>3.98</v>
       </c>
-      <c r="N15" s="48">
+      <c r="N15" s="35">
         <f t="shared" si="1"/>
         <v>3.98</v>
       </c>
-      <c r="O15" s="48"/>
-      <c r="P15" s="51" t="s">
+      <c r="O15" s="35"/>
+      <c r="P15" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="Q15" s="45" t="s">
+      <c r="Q15" s="32" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1784,27 +1781,27 @@
       <c r="H16" s="3">
         <v>1</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I16" s="20">
         <v>2576</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="21">
         <v>1.476</v>
       </c>
-      <c r="K16" s="32">
+      <c r="K16" s="19">
         <f t="shared" si="0"/>
         <v>1.476</v>
       </c>
-      <c r="L16" s="21">
+      <c r="L16" s="13">
         <v>1211</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M16" s="10">
         <v>6.4</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="15">
         <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
-      <c r="O16" s="23">
+      <c r="O16" s="15">
         <f>K16</f>
         <v>1.476</v>
       </c>
@@ -1816,50 +1813,50 @@
       </c>
     </row>
     <row r="17" spans="2:17" ht="33">
-      <c r="B17" s="37">
+      <c r="B17" s="24">
         <v>13</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="37">
+      <c r="H17" s="24">
         <v>1</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I17" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="J17" s="40" t="s">
+      <c r="J17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="41" t="s">
+      <c r="K17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="39" t="s">
+      <c r="L17" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="M17" s="40" t="s">
+      <c r="M17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="N17" s="41" t="s">
+      <c r="N17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="O17" s="41"/>
-      <c r="P17" s="42" t="s">
+      <c r="O17" s="28"/>
+      <c r="P17" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="Q17" s="43" t="s">
+      <c r="Q17" s="30" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1885,27 +1882,27 @@
       <c r="H18" s="3">
         <v>1</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="13">
         <v>0</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="10">
         <v>20.175000000000001</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="15">
         <f t="shared" si="0"/>
         <v>20.175000000000001</v>
       </c>
-      <c r="L18" s="33">
+      <c r="L18" s="20">
         <v>794</v>
       </c>
-      <c r="M18" s="34">
+      <c r="M18" s="21">
         <v>18.71</v>
       </c>
-      <c r="N18" s="32">
+      <c r="N18" s="19">
         <f t="shared" si="1"/>
         <v>18.71</v>
       </c>
-      <c r="O18" s="23">
+      <c r="O18" s="15">
         <f>N18</f>
         <v>18.71</v>
       </c>
@@ -1938,27 +1935,27 @@
       <c r="H19" s="3">
         <v>1</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="20">
         <v>17582</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J19" s="21">
         <v>0.64500000000000002</v>
       </c>
-      <c r="K19" s="32">
+      <c r="K19" s="19">
         <f t="shared" si="0"/>
         <v>0.64500000000000002</v>
       </c>
-      <c r="L19" s="21">
+      <c r="L19" s="13">
         <v>5178</v>
       </c>
-      <c r="M19" s="18">
+      <c r="M19" s="10">
         <v>1.58</v>
       </c>
-      <c r="N19" s="23">
+      <c r="N19" s="15">
         <f t="shared" si="1"/>
         <v>1.58</v>
       </c>
-      <c r="O19" s="23">
+      <c r="O19" s="15">
         <f>K19</f>
         <v>0.64500000000000002</v>
       </c>
@@ -1989,27 +1986,27 @@
       <c r="H20" s="3">
         <v>1</v>
       </c>
-      <c r="I20" s="21">
+      <c r="I20" s="13">
         <v>1</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="15">
         <f t="shared" si="0"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="L20" s="33">
+      <c r="L20" s="20">
         <v>4613</v>
       </c>
-      <c r="M20" s="34">
+      <c r="M20" s="21">
         <v>0.12</v>
       </c>
-      <c r="N20" s="32">
+      <c r="N20" s="19">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
-      <c r="O20" s="23">
+      <c r="O20" s="15">
         <f>N20</f>
         <v>0.12</v>
       </c>
@@ -2019,96 +2016,82 @@
       <c r="Q20" s="5"/>
     </row>
     <row r="21" spans="2:17">
-      <c r="B21" s="37">
+      <c r="B21" s="24">
         <v>17</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="43" t="s">
+      <c r="F21" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21" s="24">
         <v>1</v>
       </c>
-      <c r="I21" s="39" t="s">
+      <c r="I21" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="J21" s="40" t="s">
+      <c r="J21" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="K21" s="41" t="s">
+      <c r="K21" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="L21" s="39" t="s">
+      <c r="L21" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="M21" s="40" t="s">
+      <c r="M21" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="N21" s="41" t="s">
+      <c r="N21" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="O21" s="41"/>
-      <c r="P21" s="42" t="s">
+      <c r="O21" s="28"/>
+      <c r="P21" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="Q21" s="43" t="s">
+      <c r="Q21" s="30" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:17" ht="24.75" customHeight="1">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="26" t="s">
+      <c r="F22" s="16"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="M22" s="52"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="57">
+      <c r="M22" s="50"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="41">
         <f>SUM(O5:O20)</f>
         <v>38.633300000000006</v>
       </c>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="25"/>
+      <c r="Q22" s="16"/>
     </row>
     <row r="23" spans="2:17" ht="24.75" customHeight="1">
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="28"/>
+      <c r="F23" s="16"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="52"/>
       <c r="M23" s="53"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="58">
+      <c r="N23" s="54"/>
+      <c r="O23" s="42">
         <f>O22*1458.42</f>
         <v>56343.577386000012</v>
       </c>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="25"/>
+      <c r="Q23" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>